<commit_message>
css MAS tà cabando
</commit_message>
<xml_diff>
--- a/excelEXIT/excels/estoque.xlsx
+++ b/excelEXIT/excels/estoque.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
   <si>
     <t>CODIGO</t>
   </si>
@@ -47,27 +47,6 @@
   </si>
   <si>
     <t>SITUAÇÃO</t>
-  </si>
-  <si>
-    <t>goiaba</t>
-  </si>
-  <si>
-    <t>Kg</t>
-  </si>
-  <si>
-    <t>17/11/2022</t>
-  </si>
-  <si>
-    <t>02/11/2022</t>
-  </si>
-  <si>
-    <t>Disponivel</t>
-  </si>
-  <si>
-    <t>laranja</t>
-  </si>
-  <si>
-    <t>09/11/2022</t>
   </si>
   <si>
     <t>DESCRIÇÃO ITEM</t>
@@ -756,68 +735,36 @@
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:27" customHeight="1" ht="15.75">
-      <c r="B4" s="2">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
       <c r="I4" s="4">
         <f>_xlfn.DAYS(H4,G4)</f>
-        <v>-15</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J4" s="3"/>
       <c r="K4" s="2" t="str">
         <f>IF(I4&lt;=30,IF(I4&lt;=0,"Fora da Validade","Perto da Validade"),"Na Validade")</f>
         <v>Fora da Validade</v>
       </c>
     </row>
     <row r="5" spans="1:27" customHeight="1" ht="15.75">
-      <c r="B5" s="2">
-        <v>14</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.767</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="4">
         <f>_xlfn.DAYS(H5,G5)</f>
-        <v>-8</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>14</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J5" s="3"/>
       <c r="K5" s="2" t="str">
         <f>IF(I5&lt;=30,IF(I5&lt;=0,"Fora da Validade","Perto da Validade"),"Na Validade")</f>
         <v>Fora da Validade</v>
@@ -2319,13 +2266,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -2339,7 +2286,7 @@
       <c r="O2" s="14"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:26" customHeight="1" ht="15.75">
@@ -2347,40 +2294,40 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="P3" s="7" t="s">
         <v>24</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>31</v>
       </c>
       <c r="Q3" s="12"/>
     </row>
@@ -2389,10 +2336,10 @@
         <v>100001</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2">
         <v>4</v>
@@ -2440,10 +2387,10 @@
         <v>100002</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2">
         <v>5</v>
@@ -3709,16 +3656,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3752,55 +3699,55 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="17" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="17" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="17" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="K3" s="15"/>
       <c r="L3" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="M3" s="15"/>
       <c r="N3" s="17" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="17" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="Q3" s="15"/>
       <c r="R3" s="17" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="S3" s="15"/>
       <c r="T3" s="17" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="U3" s="15"/>
       <c r="V3" s="17" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="W3" s="15"/>
       <c r="X3" s="17" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="Y3" s="15"/>
       <c r="Z3" s="17" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="AA3" s="15"/>
       <c r="AB3" s="17" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="AC3" s="15"/>
       <c r="AD3" s="17" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="AE3" s="15"/>
     </row>
@@ -3810,82 +3757,82 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="Z4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="AA4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="AD4" s="7" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="AE4" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -3893,10 +3840,10 @@
         <v>100001</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E5" s="8">
         <v>9</v>
@@ -3989,10 +3936,10 @@
         <v>100002</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E6" s="8">
         <v>2.5</v>
@@ -4362,7 +4309,7 @@
     </row>
     <row r="15" spans="1:31">
       <c r="B15" s="16" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>

</xml_diff>

<commit_message>
ACABOU!!! AGORA SÓ BOTAR UM TEXTOZINHO
</commit_message>
<xml_diff>
--- a/excelEXIT/excels/estoque.xlsx
+++ b/excelEXIT/excels/estoque.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
   <si>
     <t>CODIGO</t>
   </si>
@@ -47,6 +47,21 @@
   </si>
   <si>
     <t>SITUAÇÃO</t>
+  </si>
+  <si>
+    <t>faf</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>23/11/2022</t>
+  </si>
+  <si>
+    <t>16/11/2022</t>
+  </si>
+  <si>
+    <t>Disponivel</t>
   </si>
   <si>
     <t>DESCRIÇÃO ITEM</t>
@@ -735,18 +750,34 @@
       <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:27" customHeight="1" ht="15.75">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="B4" s="2">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>3.7435</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="I4" s="4">
         <f>_xlfn.DAYS(H4,G4)</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="3"/>
+        <v>-7</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="K4" s="2" t="str">
         <f>IF(I4&lt;=30,IF(I4&lt;=0,"Fora da Validade","Perto da Validade"),"Na Validade")</f>
         <v>Fora da Validade</v>
@@ -2266,13 +2297,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
@@ -2286,7 +2317,7 @@
       <c r="O2" s="14"/>
       <c r="P2" s="15"/>
       <c r="Q2" s="11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:26" customHeight="1" ht="15.75">
@@ -2294,40 +2325,40 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="Q3" s="12"/>
     </row>
@@ -2336,10 +2367,10 @@
         <v>100001</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E4" s="2">
         <v>4</v>
@@ -2387,10 +2418,10 @@
         <v>100002</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E5" s="2">
         <v>5</v>
@@ -3656,16 +3687,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3699,55 +3730,55 @@
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="17" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="17" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="17" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K3" s="15"/>
       <c r="L3" s="17" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="M3" s="15"/>
       <c r="N3" s="17" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="O3" s="15"/>
       <c r="P3" s="17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="Q3" s="15"/>
       <c r="R3" s="17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="S3" s="15"/>
       <c r="T3" s="17" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="U3" s="15"/>
       <c r="V3" s="17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="W3" s="15"/>
       <c r="X3" s="17" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="Y3" s="15"/>
       <c r="Z3" s="17" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="AA3" s="15"/>
       <c r="AB3" s="17" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="AC3" s="15"/>
       <c r="AD3" s="17" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="AE3" s="15"/>
     </row>
@@ -3757,82 +3788,82 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="Z4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="AA4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="AD4" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="AE4" s="7" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:31">
@@ -3840,10 +3871,10 @@
         <v>100001</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E5" s="8">
         <v>9</v>
@@ -3936,10 +3967,10 @@
         <v>100002</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E6" s="8">
         <v>2.5</v>
@@ -4309,7 +4340,7 @@
     </row>
     <row r="15" spans="1:31">
       <c r="B15" s="16" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>

</xml_diff>